<commit_message>
Added minimum operating point to spine and jupyter
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA67993-1E0D-46BF-85F8-0FC80C69B251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6349F45-484C-4F55-B136-78F04EBB6B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3930" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
   <si>
     <t>Unit</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>shut_down_Output2</t>
+  </si>
+  <si>
+    <t>minimum_op_point_Output1</t>
+  </si>
+  <si>
+    <t>minimum_op_point_Output2</t>
   </si>
 </sst>
 </file>
@@ -324,9 +330,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AG6" totalsRowShown="0">
-  <autoFilter ref="A1:AG6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AI6" totalsRowShown="0">
+  <autoFilter ref="A1:AI6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="35">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
@@ -360,6 +366,8 @@
     <tableColumn id="21" xr3:uid="{400CD12D-8ADA-4557-B7CA-1464809EAFF0}" name="vom_cost_Input2"/>
     <tableColumn id="22" xr3:uid="{3FA572AD-B473-45F7-A244-2DF38E57A2D3}" name="vom_cost_Output1"/>
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
+    <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point_Output1"/>
+    <tableColumn id="35" xr3:uid="{2E0DBCBA-C50C-4413-ACD0-EC127B90A7E9}" name="minimum_op_point_Output2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -717,9 +725,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AG6"/>
+  <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -743,7 +753,7 @@
     <col min="30" max="30" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -843,8 +853,14 @@
       <c r="AG1" t="s">
         <v>57</v>
       </c>
+      <c r="AH1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -857,17 +873,26 @@
       <c r="K2">
         <v>304</v>
       </c>
+      <c r="O2">
+        <v>0.3</v>
+      </c>
+      <c r="Q2">
+        <v>0.1</v>
+      </c>
       <c r="S2">
         <v>0.5</v>
       </c>
       <c r="U2">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="AB2">
         <v>100</v>
       </c>
+      <c r="AH2">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -899,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -919,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -940,7 +965,7 @@
         <v>1.2578616352201257</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
unit_idle_heat_rate in excel + jupyter
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6349F45-484C-4F55-B136-78F04EBB6B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF33F8D-4719-4A2D-B76C-D69E322B44B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3930" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
   <si>
     <t>Unit</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>minimum_op_point_Output2</t>
+  </si>
+  <si>
+    <t>unit_idle_heat_rate</t>
   </si>
 </sst>
 </file>
@@ -330,9 +333,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AI6" totalsRowShown="0">
-  <autoFilter ref="A1:AI6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AJ6" totalsRowShown="0">
+  <autoFilter ref="A1:AJ6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
@@ -368,6 +371,7 @@
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
     <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point_Output1"/>
     <tableColumn id="35" xr3:uid="{2E0DBCBA-C50C-4413-ACD0-EC127B90A7E9}" name="minimum_op_point_Output2"/>
+    <tableColumn id="36" xr3:uid="{E8FC87F8-AAF9-461B-B88C-F56651B25838}" name="unit_idle_heat_rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -725,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,9 +755,11 @@
     <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" customWidth="1"/>
     <col min="30" max="30" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.7265625" customWidth="1"/>
+    <col min="36" max="36" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -859,8 +865,11 @@
       <c r="AI1" t="s">
         <v>72</v>
       </c>
+      <c r="AJ1" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -892,7 +901,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -923,8 +932,11 @@
       <c r="AD3">
         <v>1</v>
       </c>
+      <c r="AJ3">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -944,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -965,7 +977,7 @@
         <v>1.2578616352201257</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1014,6 +1026,9 @@
       </c>
       <c r="AA6" t="s">
         <v>61</v>
+      </c>
+      <c r="AJ6">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix incremental heat rate data prep
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF33F8D-4719-4A2D-B76C-D69E322B44B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087519F6-DD80-4DC3-ACB6-F1D102846F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AJ7" sqref="AJ7"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AJ4" sqref="AJ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -932,9 +932,6 @@
       <c r="AD3">
         <v>1</v>
       </c>
-      <c r="AJ3">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -955,6 +952,9 @@
       <c r="X4">
         <v>1</v>
       </c>
+      <c r="AJ4">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -975,6 +975,9 @@
       <c r="X5">
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
+      </c>
+      <c r="AJ5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update electrolysis data for methanol case
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087519F6-DD80-4DC3-ACB6-F1D102846F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2460A6F1-9AD4-4A1C-A027-6005A14A6F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AJ4" sqref="AJ4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -882,23 +882,8 @@
       <c r="K2">
         <v>304</v>
       </c>
-      <c r="O2">
-        <v>0.3</v>
-      </c>
-      <c r="Q2">
-        <v>0.1</v>
-      </c>
-      <c r="S2">
-        <v>0.5</v>
-      </c>
-      <c r="U2">
-        <v>0.2</v>
-      </c>
       <c r="AB2">
         <v>100</v>
-      </c>
-      <c r="AH2">
-        <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
@@ -924,13 +909,13 @@
         <v>52</v>
       </c>
       <c r="W3">
-        <v>4.7614285714285716</v>
+        <v>6.3E-3</v>
       </c>
       <c r="Y3">
-        <v>1</v>
-      </c>
-      <c r="AD3">
-        <v>1</v>
+        <v>1.76</v>
+      </c>
+      <c r="AB3">
+        <v>216.9</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update methanol reactor data
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2460A6F1-9AD4-4A1C-A027-6005A14A6F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC529E3-EE7D-422B-8B7A-E5167E1FFDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -223,9 +223,6 @@
     <t>unit_on_cost</t>
   </si>
   <si>
-    <t>0.0000001</t>
-  </si>
-  <si>
     <t>ramp_up_Output1</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t>unit_idle_heat_rate</t>
+  </si>
+  <si>
+    <t>Steam</t>
   </si>
 </sst>
 </file>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -803,28 +803,28 @@
         <v>59</v>
       </c>
       <c r="O1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" t="s">
         <v>62</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" t="s">
         <v>63</v>
       </c>
-      <c r="Q1" t="s">
-        <v>65</v>
-      </c>
-      <c r="R1" t="s">
-        <v>64</v>
-      </c>
       <c r="S1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>68</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>69</v>
-      </c>
-      <c r="V1" t="s">
-        <v>70</v>
       </c>
       <c r="W1" t="s">
         <v>39</v>
@@ -860,13 +860,13 @@
         <v>57</v>
       </c>
       <c r="AH1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI1" t="s">
         <v>71</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>72</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
@@ -948,6 +948,9 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
       <c r="D5" t="s">
         <v>24</v>
       </c>
@@ -956,6 +959,9 @@
       </c>
       <c r="J5">
         <v>52</v>
+      </c>
+      <c r="W5">
+        <v>11.03</v>
       </c>
       <c r="X5">
         <f>1/0.795</f>
@@ -982,19 +988,16 @@
         <v>22</v>
       </c>
       <c r="J6">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="K6">
         <v>100</v>
       </c>
-      <c r="L6">
-        <v>100</v>
-      </c>
       <c r="M6">
         <v>10</v>
       </c>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O6">
         <v>0.5</v>
@@ -1002,18 +1005,24 @@
       <c r="Q6">
         <v>0.5</v>
       </c>
+      <c r="S6">
+        <v>0.5</v>
+      </c>
+      <c r="U6">
+        <v>0.5</v>
+      </c>
       <c r="W6">
-        <v>1</v>
+        <v>4.57</v>
       </c>
       <c r="X6">
         <f>1/0.96</f>
         <v>1.0416666666666667</v>
       </c>
       <c r="Y6">
-        <v>4</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>61</v>
+        <v>4.32</v>
+      </c>
+      <c r="AB6">
+        <v>4.45</v>
       </c>
       <c r="AJ6">
         <v>0.1</v>

</xml_diff>

<commit_message>
integrate steam for methanol destillation
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC529E3-EE7D-422B-8B7A-E5167E1FFDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EACD116-E249-4249-AA75-B28CBB593727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -961,7 +961,7 @@
         <v>52</v>
       </c>
       <c r="W5">
-        <v>11.03</v>
+        <v>11.99</v>
       </c>
       <c r="X5">
         <f>1/0.795</f>

</xml_diff>

<commit_message>
update PV input data
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EACD116-E249-4249-AA75-B28CBB593727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2357BF5C-ED51-4D4C-905E-58A472E833CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -883,7 +883,7 @@
         <v>304</v>
       </c>
       <c r="AB2">
-        <v>100</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
@@ -915,7 +915,7 @@
         <v>1.76</v>
       </c>
       <c r="AB3">
-        <v>216.9</v>
+        <v>4.34</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update CO2 vaporizer data
assumptions made regarding power consumption
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2357BF5C-ED51-4D4C-905E-58A472E833CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30138DB8-6EAE-4D7D-95CE-425931E40093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
   <si>
     <t>Unit</t>
   </si>
@@ -732,7 +732,7 @@
   <dimension ref="A1:AJ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB17" sqref="AB17"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -925,6 +925,9 @@
       <c r="B4" t="s">
         <v>27</v>
       </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
@@ -933,6 +936,9 @@
       </c>
       <c r="K4">
         <v>100</v>
+      </c>
+      <c r="W4">
+        <v>280.5</v>
       </c>
       <c r="X4">
         <v>1</v>

</xml_diff>

<commit_message>
Add new node to solar plant if unit_idle_heat_rate is defined
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087519F6-DD80-4DC3-ACB6-F1D102846F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB2C8E7-1FE4-473F-951E-2DF40931985C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AJ4" sqref="AJ4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -898,6 +898,9 @@
         <v>100</v>
       </c>
       <c r="AH2">
+        <v>0.2</v>
+      </c>
+      <c r="AJ2">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update Model data base for methanol
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB2C8E7-1FE4-473F-951E-2DF40931985C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30138DB8-6EAE-4D7D-95CE-425931E40093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
   <si>
     <t>Unit</t>
   </si>
@@ -223,9 +223,6 @@
     <t>unit_on_cost</t>
   </si>
   <si>
-    <t>0.0000001</t>
-  </si>
-  <si>
     <t>ramp_up_Output1</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t>unit_idle_heat_rate</t>
+  </si>
+  <si>
+    <t>Steam</t>
   </si>
 </sst>
 </file>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -803,28 +803,28 @@
         <v>59</v>
       </c>
       <c r="O1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" t="s">
         <v>62</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" t="s">
         <v>63</v>
       </c>
-      <c r="Q1" t="s">
-        <v>65</v>
-      </c>
-      <c r="R1" t="s">
-        <v>64</v>
-      </c>
       <c r="S1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>68</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>69</v>
-      </c>
-      <c r="V1" t="s">
-        <v>70</v>
       </c>
       <c r="W1" t="s">
         <v>39</v>
@@ -860,13 +860,13 @@
         <v>57</v>
       </c>
       <c r="AH1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI1" t="s">
         <v>71</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>72</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
@@ -882,26 +882,8 @@
       <c r="K2">
         <v>304</v>
       </c>
-      <c r="O2">
-        <v>0.3</v>
-      </c>
-      <c r="Q2">
-        <v>0.1</v>
-      </c>
-      <c r="S2">
-        <v>0.5</v>
-      </c>
-      <c r="U2">
-        <v>0.2</v>
-      </c>
       <c r="AB2">
-        <v>100</v>
-      </c>
-      <c r="AH2">
-        <v>0.2</v>
-      </c>
-      <c r="AJ2">
-        <v>0.2</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
@@ -927,13 +909,13 @@
         <v>52</v>
       </c>
       <c r="W3">
-        <v>4.7614285714285716</v>
+        <v>6.3E-3</v>
       </c>
       <c r="Y3">
-        <v>1</v>
-      </c>
-      <c r="AD3">
-        <v>1</v>
+        <v>1.76</v>
+      </c>
+      <c r="AB3">
+        <v>4.34</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
@@ -943,6 +925,9 @@
       <c r="B4" t="s">
         <v>27</v>
       </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
@@ -951,6 +936,9 @@
       </c>
       <c r="K4">
         <v>100</v>
+      </c>
+      <c r="W4">
+        <v>280.5</v>
       </c>
       <c r="X4">
         <v>1</v>
@@ -966,6 +954,9 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
       <c r="D5" t="s">
         <v>24</v>
       </c>
@@ -974,6 +965,9 @@
       </c>
       <c r="J5">
         <v>52</v>
+      </c>
+      <c r="W5">
+        <v>11.99</v>
       </c>
       <c r="X5">
         <f>1/0.795</f>
@@ -1000,19 +994,16 @@
         <v>22</v>
       </c>
       <c r="J6">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="K6">
         <v>100</v>
       </c>
-      <c r="L6">
-        <v>100</v>
-      </c>
       <c r="M6">
         <v>10</v>
       </c>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O6">
         <v>0.5</v>
@@ -1020,18 +1011,24 @@
       <c r="Q6">
         <v>0.5</v>
       </c>
+      <c r="S6">
+        <v>0.5</v>
+      </c>
+      <c r="U6">
+        <v>0.5</v>
+      </c>
       <c r="W6">
-        <v>1</v>
+        <v>4.57</v>
       </c>
       <c r="X6">
         <f>1/0.96</f>
         <v>1.0416666666666667</v>
       </c>
       <c r="Y6">
-        <v>4</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>61</v>
+        <v>4.32</v>
+      </c>
+      <c r="AB6">
+        <v>4.45</v>
       </c>
       <c r="AJ6">
         <v>0.1</v>

</xml_diff>

<commit_message>
Error message if min op point but no capacity given
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30138DB8-6EAE-4D7D-95CE-425931E40093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA544A48-F368-41BB-B06D-38FE1546151A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
   <si>
     <t>Unit</t>
   </si>
@@ -250,23 +250,23 @@
     <t>shut_down_Output2</t>
   </si>
   <si>
-    <t>minimum_op_point_Output1</t>
-  </si>
-  <si>
-    <t>minimum_op_point_Output2</t>
-  </si>
-  <si>
     <t>unit_idle_heat_rate</t>
   </si>
   <si>
     <t>Steam</t>
+  </si>
+  <si>
+    <t>minimum_op_point</t>
+  </si>
+  <si>
+    <t>Error messages:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +276,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -301,13 +308,74 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -369,9 +437,11 @@
     <tableColumn id="21" xr3:uid="{400CD12D-8ADA-4557-B7CA-1464809EAFF0}" name="vom_cost_Input2"/>
     <tableColumn id="22" xr3:uid="{3FA572AD-B473-45F7-A244-2DF38E57A2D3}" name="vom_cost_Output1"/>
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
-    <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point_Output1"/>
-    <tableColumn id="35" xr3:uid="{2E0DBCBA-C50C-4413-ACD0-EC127B90A7E9}" name="minimum_op_point_Output2"/>
+    <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point"/>
     <tableColumn id="36" xr3:uid="{E8FC87F8-AAF9-461B-B88C-F56651B25838}" name="unit_idle_heat_rate"/>
+    <tableColumn id="37" xr3:uid="{EE9BC032-0112-449B-9748-951DE19178CE}" name="Error messages:" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -386,7 +456,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -415,7 +485,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:J5" totalsRowShown="0">
   <autoFilter ref="A1:J5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="7">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="value_before"/>
@@ -729,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AJ6"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -756,7 +826,8 @@
     <col min="29" max="29" width="11" customWidth="1"/>
     <col min="30" max="30" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8.7265625" customWidth="1"/>
-    <col min="36" max="36" width="19" customWidth="1"/>
+    <col min="35" max="35" width="19" customWidth="1"/>
+    <col min="36" max="36" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
@@ -860,13 +931,13 @@
         <v>57</v>
       </c>
       <c r="AH1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI1" t="s">
         <v>70</v>
       </c>
-      <c r="AI1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>72</v>
+      <c r="AJ1" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
@@ -876,14 +947,18 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="J2">
-        <v>304</v>
-      </c>
       <c r="K2">
         <v>304</v>
       </c>
+      <c r="L2">
+        <v>304</v>
+      </c>
       <c r="AB2">
         <v>1.29</v>
+      </c>
+      <c r="AJ2" s="1" t="str">
+        <f>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</f>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.35">
@@ -917,6 +992,10 @@
       <c r="AB3">
         <v>4.34</v>
       </c>
+      <c r="AJ3" s="1" t="str">
+        <f>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -943,8 +1022,12 @@
       <c r="X4">
         <v>1</v>
       </c>
-      <c r="AJ4">
+      <c r="AI4">
         <v>0.1</v>
+      </c>
+      <c r="AJ4" s="1" t="str">
+        <f>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</f>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
@@ -955,7 +1038,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -973,8 +1056,12 @@
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
-      <c r="AJ5">
+      <c r="AI5">
         <v>0.1</v>
+      </c>
+      <c r="AJ5" s="1" t="str">
+        <f>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.35">
@@ -1030,8 +1117,21 @@
       <c r="AB6">
         <v>4.45</v>
       </c>
-      <c r="AJ6">
+      <c r="AI6">
         <v>0.1</v>
+      </c>
+      <c r="AJ6" s="1" t="str">
+        <f>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f>IF(COUNTBLANK(AJ2:AJ6)&lt;&gt;ROWS(AJ2:AJ6),"Please check error message on the right","")</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed minimum operating point to capacity node + warning message in excel
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA544A48-F368-41BB-B06D-38FE1546151A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7836D1-D6D4-4896-AA0D-4D6F83BE74FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
   <si>
     <t>Unit</t>
   </si>
@@ -266,7 +266,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +286,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -308,14 +314,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -333,59 +351,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -439,8 +404,8 @@
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
     <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point"/>
     <tableColumn id="36" xr3:uid="{E8FC87F8-AAF9-461B-B88C-F56651B25838}" name="unit_idle_heat_rate"/>
-    <tableColumn id="37" xr3:uid="{EE9BC032-0112-449B-9748-951DE19178CE}" name="Error messages:" dataDxfId="0">
-      <calculatedColumnFormula>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</calculatedColumnFormula>
+    <tableColumn id="37" xr3:uid="{EE9BC032-0112-449B-9748-951DE19178CE}" name="Error messages:" dataDxfId="2">
+      <calculatedColumnFormula>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -456,7 +421,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="8"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -485,7 +450,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:J5" totalsRowShown="0">
   <autoFilter ref="A1:J5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="value_before"/>
@@ -802,7 +767,7 @@
   <dimension ref="A1:AJ9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,7 +792,7 @@
     <col min="30" max="30" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8.7265625" customWidth="1"/>
     <col min="35" max="35" width="19" customWidth="1"/>
-    <col min="36" max="36" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
@@ -947,17 +912,20 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
+      <c r="J2">
+        <v>304</v>
+      </c>
       <c r="K2">
         <v>304</v>
       </c>
-      <c r="L2">
-        <v>304</v>
-      </c>
       <c r="AB2">
         <v>1.29</v>
       </c>
-      <c r="AJ2" s="1" t="str">
-        <f>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</f>
+      <c r="AH2">
+        <v>0.5</v>
+      </c>
+      <c r="AJ2" s="2" t="str">
+        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
@@ -992,8 +960,11 @@
       <c r="AB3">
         <v>4.34</v>
       </c>
-      <c r="AJ3" s="1" t="str">
-        <f>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</f>
+      <c r="AH3">
+        <v>0.5</v>
+      </c>
+      <c r="AJ3" s="2" t="str">
+        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
@@ -1022,11 +993,14 @@
       <c r="X4">
         <v>1</v>
       </c>
+      <c r="AH4">
+        <v>0.2</v>
+      </c>
       <c r="AI4">
         <v>0.1</v>
       </c>
-      <c r="AJ4" s="1" t="str">
-        <f>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</f>
+      <c r="AJ4" s="2" t="str">
+        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
@@ -1059,8 +1033,8 @@
       <c r="AI5">
         <v>0.1</v>
       </c>
-      <c r="AJ5" s="1" t="str">
-        <f>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</f>
+      <c r="AJ5" s="2" t="str">
+        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
@@ -1120,25 +1094,20 @@
       <c r="AI6">
         <v>0.1</v>
       </c>
-      <c r="AJ6" s="1" t="str">
-        <f>IF(Table1[[#This Row],[minimum_op_point]]&lt;&gt;"",IF(AND(ISBLANK(Table1[[#This Row],[Cap_Input1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Input2_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output1_existing]]),ISBLANK(Table1[[#This Row],[Cap_Output2_existing]])),"no capacity is given",""),"")</f>
+      <c r="AJ6" s="2" t="str">
+        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="1" t="str">
-        <f>IF(COUNTBLANK(AJ2:AJ6)&lt;&gt;ROWS(AJ2:AJ6),"Please check error message on the right","")</f>
-        <v/>
-      </c>
+      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update fix relation power to water for PEM
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA48EC2D-BB8E-4BAB-922C-07B6C57B1583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54C9C77-E74A-4501-9E09-6DD59E4C315B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -767,7 +767,7 @@
   <dimension ref="A1:AJ9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AH4" sqref="AH4"/>
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -949,7 +949,7 @@
         <v>52</v>
       </c>
       <c r="W3">
-        <v>6.3E-3</v>
+        <v>5.8500000000000002E-3</v>
       </c>
       <c r="Y3">
         <v>1.76</v>

</xml_diff>

<commit_message>
fix missing relation bug
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772AF23C-1873-4292-9CDC-753E54F5F003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7C9A72-B5B5-4637-9CB4-6AF5ED637E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1256,6 +1256,9 @@
       </c>
       <c r="N2">
         <v>1000</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
       </c>
       <c r="S2">
         <v>1</v>

</xml_diff>

<commit_message>
Corrected incremental heat rate
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7C9A72-B5B5-4637-9CB4-6AF5ED637E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{CD7C9A72-B5B5-4637-9CB4-6AF5ED637E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC3A9CA2-BE72-4347-B037-4D46E66EC1AD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
   <si>
     <t>Unit</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>Error messages:</t>
+  </si>
+  <si>
+    <t>Steam_Plant</t>
   </si>
 </sst>
 </file>
@@ -366,8 +369,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AJ6" totalsRowShown="0">
-  <autoFilter ref="A1:AJ6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AJ7" totalsRowShown="0">
+  <autoFilter ref="A1:AJ7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
   <tableColumns count="36">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
@@ -766,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1093,6 +1096,30 @@
         <v/>
       </c>
     </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7">
+        <v>200</v>
+      </c>
+      <c r="W7">
+        <v>0.2</v>
+      </c>
+      <c r="AJ7" s="1" t="str">
+        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
+        <v/>
+      </c>
+    </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
     </row>
@@ -1110,7 +1137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Created function for adjusted efficiency
+ now takes mean_value from model data base and does the whole charade in one step. Not quite finished yet, but good enough so one (I) can continue tomorrow with the rest of the df_variable_efficiency
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{CD7C9A72-B5B5-4637-9CB4-6AF5ED637E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A475E2DF-F9D7-48C7-AE6D-122D09AB0AC5}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{CD7C9A72-B5B5-4637-9CB4-6AF5ED637E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B818528D-BFC2-4302-BACA-2E876E13705B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -17,6 +17,40 @@
     <sheet name="Connections" sheetId="2" r:id="rId2"/>
     <sheet name="Storages" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="CIQWBGuid" hidden="1">"d2034e36-8705-4dfd-a632-cd174c2c5e1f"</definedName>
+    <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
+    <definedName name="IQ_CH">110000</definedName>
+    <definedName name="IQ_CQ">5000</definedName>
+    <definedName name="IQ_CY">10000</definedName>
+    <definedName name="IQ_DAILY">500000</definedName>
+    <definedName name="IQ_DNTM" hidden="1">700000</definedName>
+    <definedName name="IQ_FH">100000</definedName>
+    <definedName name="IQ_FQ">500</definedName>
+    <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
+    <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
+    <definedName name="IQ_FWD_CY2" hidden="1">10003</definedName>
+    <definedName name="IQ_FWD_FY" hidden="1">1001</definedName>
+    <definedName name="IQ_FWD_FY1" hidden="1">1002</definedName>
+    <definedName name="IQ_FWD_FY2" hidden="1">1003</definedName>
+    <definedName name="IQ_FWD_Q" hidden="1">501</definedName>
+    <definedName name="IQ_FWD_Q1" hidden="1">502</definedName>
+    <definedName name="IQ_FWD_Q2" hidden="1">503</definedName>
+    <definedName name="IQ_FY">1000</definedName>
+    <definedName name="IQ_LATESTK" hidden="1">1000</definedName>
+    <definedName name="IQ_LATESTQ" hidden="1">500</definedName>
+    <definedName name="IQ_LTM">2000</definedName>
+    <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
+    <definedName name="IQ_MONTH">15000</definedName>
+    <definedName name="IQ_MTD" hidden="1">800000</definedName>
+    <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">45429.7589699074</definedName>
+    <definedName name="IQ_NTM">6000</definedName>
+    <definedName name="IQ_QTD" hidden="1">750000</definedName>
+    <definedName name="IQ_TODAY" hidden="1">0</definedName>
+    <definedName name="IQ_WEEK">50000</definedName>
+    <definedName name="IQ_YTD">3000</definedName>
+    <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t>Unit</t>
   </si>
@@ -263,6 +297,9 @@
   </si>
   <si>
     <t>Steam_Plant</t>
+  </si>
+  <si>
+    <t>mean_efficiency</t>
   </si>
 </sst>
 </file>
@@ -327,6 +364,17 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -344,17 +392,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -369,9 +406,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AJ7" totalsRowShown="0">
-  <autoFilter ref="A1:AJ7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AK7" totalsRowShown="0">
+  <autoFilter ref="A1:AK7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="37">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
@@ -385,6 +422,7 @@
     <tableColumn id="17" xr3:uid="{6408F114-841E-472E-92F5-7B63FF1B66F4}" name="Cap_Output_1_max"/>
     <tableColumn id="18" xr3:uid="{541C17F0-C020-47FE-9DA4-DB76D7416668}" name="Cap_Output2_existing"/>
     <tableColumn id="19" xr3:uid="{D6FEE63D-DC89-4D1A-9708-5E7C70FD5793}" name="Cap_Output2_max"/>
+    <tableColumn id="35" xr3:uid="{C3887B4E-C4A5-42AB-A92F-97AD44212E95}" name="mean_efficiency"/>
     <tableColumn id="8" xr3:uid="{5F719CEE-A0F7-452C-B82C-E739C5FED49B}" name="min_down_time"/>
     <tableColumn id="26" xr3:uid="{D0F85E7B-D704-45A0-BE99-26E3A1F08634}" name="ramp_up_Output1"/>
     <tableColumn id="28" xr3:uid="{EBC4610B-47F0-44E3-8543-664851FC473C}" name="ramp_up_Output2"/>
@@ -407,7 +445,7 @@
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
     <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point"/>
     <tableColumn id="36" xr3:uid="{E8FC87F8-AAF9-461B-B88C-F56651B25838}" name="unit_idle_heat_rate"/>
-    <tableColumn id="37" xr3:uid="{EE9BC032-0112-449B-9748-951DE19178CE}" name="Error messages:" dataDxfId="0">
+    <tableColumn id="37" xr3:uid="{EE9BC032-0112-449B-9748-951DE19178CE}" name="Error messages:" dataDxfId="2">
       <calculatedColumnFormula>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -424,7 +462,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -453,7 +491,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:J5" totalsRowShown="0">
   <autoFilter ref="A1:J5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="value_before"/>
@@ -471,9 +509,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -511,7 +549,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -617,7 +655,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -759,7 +797,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -767,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AJ9"/>
+  <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AB17" sqref="AB17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -784,21 +822,22 @@
     <col min="10" max="10" width="21.90625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.08984375" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" hidden="1" customWidth="1"/>
-    <col min="14" max="22" width="10.54296875" customWidth="1"/>
-    <col min="23" max="23" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="12.7265625" customWidth="1"/>
-    <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11" customWidth="1"/>
-    <col min="30" max="30" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.7265625" customWidth="1"/>
-    <col min="35" max="35" width="19" customWidth="1"/>
-    <col min="36" max="36" width="17.36328125" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="23" width="10.54296875" customWidth="1"/>
+    <col min="24" max="24" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="12.7265625" customWidth="1"/>
+    <col min="29" max="29" width="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.7265625" customWidth="1"/>
+    <col min="36" max="36" width="19" customWidth="1"/>
+    <col min="37" max="37" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -839,76 +878,79 @@
         <v>35</v>
       </c>
       <c r="N1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" t="s">
         <v>59</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>61</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>64</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>63</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>66</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>67</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>68</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>69</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>39</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>60</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>54</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>58</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>57</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>72</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>70</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -921,19 +963,19 @@
       <c r="K2">
         <v>304</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <f>Table1[[#This Row],[Cap_Output1_existing]]*0.56</f>
         <v>170.24</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>1.29</v>
       </c>
-      <c r="AJ2" s="2" t="str">
+      <c r="AK2" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -955,24 +997,27 @@
       <c r="G3">
         <v>52</v>
       </c>
-      <c r="W3">
+      <c r="N3">
+        <v>0.6</v>
+      </c>
+      <c r="X3">
         <v>5.8500000000000002E-3</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>1.76</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>4.34</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>0.19</v>
       </c>
-      <c r="AJ3" s="2" t="str">
+      <c r="AK3" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -991,21 +1036,21 @@
       <c r="K4">
         <v>100</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>280.5</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>1</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>0.1</v>
       </c>
-      <c r="AJ4" s="2" t="str">
+      <c r="AK4" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1024,22 +1069,22 @@
       <c r="J5">
         <v>52</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>11.99</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>0.1</v>
       </c>
-      <c r="AJ5" s="2" t="str">
+      <c r="AK5" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1064,43 +1109,46 @@
       <c r="M6">
         <v>10</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6">
+        <v>0.7</v>
+      </c>
+      <c r="O6" t="s">
         <v>65</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.5</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>0.5</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>0.5</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>0.5</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>4.57</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <f>1/0.96</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>4.32</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>4.45</v>
       </c>
-      <c r="AI6">
+      <c r="AJ6">
         <v>0.1</v>
       </c>
-      <c r="AJ6" s="2" t="str">
+      <c r="AK6" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -1116,15 +1164,15 @@
       <c r="J7">
         <v>200</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>0.2</v>
       </c>
-      <c r="AJ7" s="1" t="str">
+      <c r="AK7" s="1" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update raw input data to new mapping
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FCC1DD-E064-4774-822D-3D8D47CE3790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C302134D-1196-4EA9-A3F5-88A0BBFD1335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -1189,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1362,6 +1362,9 @@
       <c r="F3" t="s">
         <v>60</v>
       </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
       <c r="I3">
         <v>1000</v>
       </c>
@@ -1372,6 +1375,9 @@
         <v>1000</v>
       </c>
       <c r="L3">
+        <v>1000</v>
+      </c>
+      <c r="M3">
         <v>1000</v>
       </c>
       <c r="S3">
@@ -1397,6 +1403,9 @@
       <c r="F4" t="s">
         <v>60</v>
       </c>
+      <c r="G4">
+        <v>1000</v>
+      </c>
       <c r="I4">
         <v>1000</v>
       </c>
@@ -1407,6 +1416,9 @@
         <v>1000</v>
       </c>
       <c r="L4">
+        <v>1000</v>
+      </c>
+      <c r="M4">
         <v>1000</v>
       </c>
       <c r="S4">
@@ -1455,7 +1467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add a CO2 price to the inputs
price is variable cost for the CO2 vaporizer
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C302134D-1196-4EA9-A3F5-88A0BBFD1335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32411B78-865A-413B-8515-4A971BDF562A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1042,6 +1042,9 @@
       <c r="Y4">
         <v>1</v>
       </c>
+      <c r="AE4">
+        <v>26.81</v>
+      </c>
       <c r="AJ4">
         <v>0.1</v>
       </c>
@@ -1189,7 +1192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add hydrogen storage loss rate
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C33584E-37B2-424E-AAE6-06E24AF88072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349D3A1B-70EA-45BB-BA2E-E19B9F23EB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1471,7 +1471,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1534,7 +1534,7 @@
         <v>5478.6764505058327</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>4.147E-2</v>
       </c>
       <c r="G2" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
add hydrogen storage round trip efficiency
represent the losses for injection and rejection.
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349D3A1B-70EA-45BB-BA2E-E19B9F23EB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9892C506-773E-4F3B-8F5F-F19E7A693515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -1192,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1384,7 +1384,7 @@
         <v>1000</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
@@ -1470,7 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add hydrogen storage fom cost to input
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9892C506-773E-4F3B-8F5F-F19E7A693515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F8415D-C0A8-431C-9D52-EED5941C19C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AA11" sqref="AA11"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Y35" sqref="Y35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1193,7 +1193,7 @@
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1385,6 +1385,9 @@
       </c>
       <c r="S3">
         <v>0.88</v>
+      </c>
+      <c r="U3">
+        <v>7.2835616438356163E-2</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update input data with electric boiler info
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F8415D-C0A8-431C-9D52-EED5941C19C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F4251A-F72A-472B-8361-D891D1F2895F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y35" sqref="Y35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1073,7 +1073,7 @@
         <v>52</v>
       </c>
       <c r="X5">
-        <v>11.99</v>
+        <v>7.9901515151515144E-3</v>
       </c>
       <c r="Y5">
         <f>1/0.795</f>
@@ -1156,19 +1156,28 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
         <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
       </c>
-      <c r="J7">
-        <v>200</v>
+      <c r="F7">
+        <v>100</v>
       </c>
       <c r="X7">
-        <v>0.2</v>
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>0.99</v>
+      </c>
+      <c r="AC7">
+        <v>0.11929223744292237</v>
+      </c>
+      <c r="AJ7">
+        <v>0.1</v>
       </c>
       <c r="AK7" s="1" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
@@ -1192,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add water cost to model input sheet
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F4251A-F72A-472B-8361-D891D1F2895F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0E04C5-D855-4560-B9A5-72D0722CFE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -808,7 +808,7 @@
   <dimension ref="A1:AK9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1009,6 +1009,9 @@
       <c r="AC3">
         <v>4.34</v>
       </c>
+      <c r="AF3">
+        <v>1.4865951742627346</v>
+      </c>
       <c r="AI3">
         <v>0.19</v>
       </c>
@@ -1175,6 +1178,9 @@
       </c>
       <c r="AC7">
         <v>0.11929223744292237</v>
+      </c>
+      <c r="AF7">
+        <v>1.4865951742627346</v>
       </c>
       <c r="AJ7">
         <v>0.1</v>

</xml_diff>

<commit_message>
update model data base
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0E04C5-D855-4560-B9A5-72D0722CFE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD31BF8-3695-4071-BBDF-29FF9196858E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1076,7 +1076,7 @@
         <v>52</v>
       </c>
       <c r="X5">
-        <v>7.9901515151515144E-3</v>
+        <v>10.273051948051947</v>
       </c>
       <c r="Y5">
         <f>1/0.795</f>

</xml_diff>

<commit_message>
change order ot inputs for CO2 vaporizer
necessary to be in line with the data prep routines
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD31BF8-3695-4071-BBDF-29FF9196858E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D85E59-02C2-41A6-B4E0-D93DE2B5F476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-3300" yWindow="-19950" windowWidth="28800" windowHeight="15225" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -808,7 +808,7 @@
   <dimension ref="A1:AK9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1025,10 +1025,10 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
         <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
       </c>
       <c r="D4" t="s">
         <v>45</v>
@@ -1040,10 +1040,10 @@
         <v>100</v>
       </c>
       <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
         <v>280.5</v>
-      </c>
-      <c r="Y4">
-        <v>1</v>
       </c>
       <c r="AE4">
         <v>26.81</v>
@@ -1208,7 +1208,7 @@
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1489,7 +1489,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update steam to raw methonal ratio in data base
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D85E59-02C2-41A6-B4E0-D93DE2B5F476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBB2979-11F4-4ED2-9248-6B471ED2E00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3300" yWindow="-19950" windowWidth="28800" windowHeight="15225" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -808,7 +808,7 @@
   <dimension ref="A1:AK9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1076,7 +1076,7 @@
         <v>52</v>
       </c>
       <c r="X5">
-        <v>10.273051948051947</v>
+        <v>17.277901743828668</v>
       </c>
       <c r="Y5">
         <f>1/0.795</f>

</xml_diff>

<commit_message>
update water cost to euro/l in data base
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBB2979-11F4-4ED2-9248-6B471ED2E00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BC8720-1F6E-44C9-B03D-6E29CD1EEB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3300" yWindow="-19950" windowWidth="28800" windowHeight="15225" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AG21" sqref="AG21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1010,7 +1010,7 @@
         <v>4.34</v>
       </c>
       <c r="AF3">
-        <v>1.4865951742627346</v>
+        <v>1.4865951742627345E-3</v>
       </c>
       <c r="AI3">
         <v>0.19</v>
@@ -1180,7 +1180,7 @@
         <v>0.11929223744292237</v>
       </c>
       <c r="AF7">
-        <v>1.4865951742627346</v>
+        <v>1.4865951742627345E-3</v>
       </c>
       <c r="AJ7">
         <v>0.1</v>

</xml_diff>

<commit_message>
update steam unit parameters in data base
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BC8720-1F6E-44C9-B03D-6E29CD1EEB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13C8ED2-2FB4-4199-AE44-DECB0E221A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3300" yWindow="-19950" windowWidth="28800" windowHeight="15225" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AG21" sqref="AG21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1171,7 +1171,7 @@
         <v>100</v>
       </c>
       <c r="X7">
-        <v>1</v>
+        <v>7.2437800000000002E-4</v>
       </c>
       <c r="Y7">
         <v>0.99</v>

</xml_diff>

<commit_message>
update relation values in model data base
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13C8ED2-2FB4-4199-AE44-DECB0E221A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5002E8D-78E9-4C11-9177-43D5EECB13D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -808,7 +808,7 @@
   <dimension ref="A1:AK9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1134,7 +1134,7 @@
         <v>0.5</v>
       </c>
       <c r="X6">
-        <v>4.57</v>
+        <v>3.4889142857142859</v>
       </c>
       <c r="Y6">
         <f>1/0.96</f>

</xml_diff>

<commit_message>
update h2 to co2 input ration in data base
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5002E8D-78E9-4C11-9177-43D5EECB13D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FE0305-849E-4F72-B812-E690CBB20E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -808,7 +808,7 @@
   <dimension ref="A1:AK9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1040,10 +1040,10 @@
         <v>100</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>3.6010731197896975E-3</v>
       </c>
       <c r="Y4">
-        <v>280.5</v>
+        <v>0.99</v>
       </c>
       <c r="AE4">
         <v>26.81</v>
@@ -1134,7 +1134,7 @@
         <v>0.5</v>
       </c>
       <c r="X6">
-        <v>3.4889142857142859</v>
+        <v>5.1734967222388608</v>
       </c>
       <c r="Y6">
         <f>1/0.96</f>

</xml_diff>

<commit_message>
update co2 vaporizer relations in data base
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FE0305-849E-4F72-B812-E690CBB20E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8321FB60-B687-4E86-A150-DE1458205CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1043,7 +1043,7 @@
         <v>3.6010731197896975E-3</v>
       </c>
       <c r="Y4">
-        <v>0.99</v>
+        <v>3.601073119789697E-3</v>
       </c>
       <c r="AE4">
         <v>26.81</v>

</xml_diff>

<commit_message>
update methanol storage efficiencies in data base
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8321FB60-B687-4E86-A150-DE1458205CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBB6B4D-1557-49D8-974C-DE9B9750203A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -354,10 +354,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,7 +809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
@@ -1207,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1442,8 +1444,11 @@
       <c r="M4">
         <v>1000</v>
       </c>
-      <c r="S4">
-        <v>1</v>
+      <c r="Q4" s="3">
+        <v>0.99983999999999995</v>
+      </c>
+      <c r="S4" s="4">
+        <v>0.99983999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update methanol storage fom and investment cost
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBB6B4D-1557-49D8-974C-DE9B9750203A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0450BA5-F4D8-4B3A-85C0-8E614B782A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -354,12 +354,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1232,7 +1230,7 @@
     <col min="18" max="18" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.81640625" customWidth="1"/>
     <col min="20" max="20" width="12.7265625" customWidth="1"/>
-    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.81640625" customWidth="1"/>
     <col min="22" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1444,11 +1442,14 @@
       <c r="M4">
         <v>1000</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4">
         <v>0.99983999999999995</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S4">
         <v>0.99983999999999995</v>
+      </c>
+      <c r="U4">
+        <v>1.0958904109589041E-2</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
@@ -1483,8 +1484,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1494,7 +1496,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated Model Base (temporal slicing + electrolyzer)
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0450BA5-F4D8-4B3A-85C0-8E614B782A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{B0450BA5-F4D8-4B3A-85C0-8E614B782A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01E7CA9A-FE0B-4E20-A50F-9C1D62B5D954}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Storages" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"d2034e36-8705-4dfd-a632-cd174c2c5e1f"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"b590661c-45e2-4f13-b772-b3756cc39e58"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
   <si>
     <t>Unit</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>fix_node_state</t>
+  </si>
+  <si>
+    <t>resolution_output</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -354,15 +360,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -392,6 +401,9 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -405,10 +417,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AK7" totalsRowShown="0">
-  <autoFilter ref="A1:AK7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AL7" totalsRowShown="0">
+  <autoFilter ref="A1:AL7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="38">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
@@ -445,6 +461,7 @@
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
     <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point"/>
     <tableColumn id="36" xr3:uid="{E8FC87F8-AAF9-461B-B88C-F56651B25838}" name="unit_idle_heat_rate"/>
+    <tableColumn id="39" xr3:uid="{52BB7FF5-8204-4DA8-90EB-65B1611ED0E8}" name="resolution_output" dataDxfId="3"/>
     <tableColumn id="37" xr3:uid="{EE9BC032-0112-449B-9748-951DE19178CE}" name="Error messages:" dataDxfId="2">
       <calculatedColumnFormula>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</calculatedColumnFormula>
     </tableColumn>
@@ -805,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AK9"/>
+  <dimension ref="A1:AL9"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -834,10 +851,11 @@
     <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="8.7265625" customWidth="1"/>
     <col min="36" max="36" width="19" customWidth="1"/>
-    <col min="37" max="37" width="17.453125" customWidth="1"/>
+    <col min="37" max="37" width="18" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -946,11 +964,14 @@
       <c r="AJ1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -970,12 +991,13 @@
       <c r="AC2">
         <v>1.29</v>
       </c>
-      <c r="AK2" s="2" t="str">
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -998,7 +1020,7 @@
         <v>52</v>
       </c>
       <c r="N3">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="X3">
         <v>5.8500000000000002E-3</v>
@@ -1015,12 +1037,13 @@
       <c r="AI3">
         <v>0.19</v>
       </c>
-      <c r="AK3" s="2" t="str">
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1051,12 +1074,13 @@
       <c r="AJ4">
         <v>0.1</v>
       </c>
-      <c r="AK4" s="2" t="str">
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1085,12 +1109,15 @@
       <c r="AJ5">
         <v>0.1</v>
       </c>
-      <c r="AK5" s="2" t="str">
+      <c r="AK5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL5" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1149,12 +1176,13 @@
       <c r="AJ6">
         <v>0.1</v>
       </c>
-      <c r="AK6" s="2" t="str">
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1185,16 +1213,22 @@
       <c r="AJ7">
         <v>0.1</v>
       </c>
-      <c r="AK7" s="1" t="str">
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="1" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK2:AK7" xr:uid="{8771E67A-C02C-457D-9686-E902BF0F8B2C}">
+      <formula1>"h, D, W, Q, M, Y"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1207,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated database for temporal slicing
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B4E73A-EA77-4643-B0C9-9E0954A17787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{40B4E73A-EA77-4643-B0C9-9E0954A17787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C45DE6B2-903C-4C80-9498-10EAA20BD3F1}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Storages" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"d2034e36-8705-4dfd-a632-cd174c2c5e1f"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"210897e0-4881-414f-bd24-48d4d4bcce74"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
   <si>
     <t>Unit</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>fix_node_state</t>
+  </si>
+  <si>
+    <t>resolution_output</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -354,25 +360,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -392,6 +393,17 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -406,9 +418,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AK7" totalsRowShown="0">
-  <autoFilter ref="A1:AK7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AL7" totalsRowShown="0">
+  <autoFilter ref="A1:AL7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="38">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
@@ -445,7 +457,8 @@
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
     <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point"/>
     <tableColumn id="36" xr3:uid="{E8FC87F8-AAF9-461B-B88C-F56651B25838}" name="unit_idle_heat_rate"/>
-    <tableColumn id="37" xr3:uid="{EE9BC032-0112-449B-9748-951DE19178CE}" name="Error messages:" dataDxfId="2">
+    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="0"/>
+    <tableColumn id="37" xr3:uid="{EE9BC032-0112-449B-9748-951DE19178CE}" name="Error messages:" dataDxfId="1">
       <calculatedColumnFormula>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -462,7 +475,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -491,7 +504,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:J5" totalsRowShown="0">
   <autoFilter ref="A1:J5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="2">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="value_before"/>
@@ -805,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AK9"/>
+  <dimension ref="A1:AL9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AJ11" sqref="AJ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -834,10 +847,11 @@
     <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="8.7265625" customWidth="1"/>
     <col min="36" max="36" width="19" customWidth="1"/>
-    <col min="37" max="37" width="17.453125" customWidth="1"/>
+    <col min="37" max="37" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -946,11 +960,14 @@
       <c r="AJ1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -970,12 +987,13 @@
       <c r="AC2">
         <v>1.29</v>
       </c>
-      <c r="AK2" s="2" t="str">
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1015,12 +1033,13 @@
       <c r="AI3">
         <v>0.19</v>
       </c>
-      <c r="AK3" s="2" t="str">
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1051,12 +1070,13 @@
       <c r="AJ4">
         <v>0.1</v>
       </c>
-      <c r="AK4" s="2" t="str">
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1085,12 +1105,15 @@
       <c r="AJ5">
         <v>0.1</v>
       </c>
-      <c r="AK5" s="2" t="str">
+      <c r="AK5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL5" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1149,12 +1172,13 @@
       <c r="AJ6">
         <v>0.1</v>
       </c>
-      <c r="AK6" s="2" t="str">
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1185,16 +1209,22 @@
       <c r="AJ7">
         <v>0.1</v>
       </c>
-      <c r="AK7" s="1" t="str">
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="1" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK2:AK7" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
+      <formula1>"h, D, W, M, Q, Y"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Updated everything for changed demand for end product
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{40B4E73A-EA77-4643-B0C9-9E0954A17787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C45DE6B2-903C-4C80-9498-10EAA20BD3F1}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{40B4E73A-EA77-4643-B0C9-9E0954A17787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{350DF377-31C5-4078-A49F-3DF2DBA61E28}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Storages" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"210897e0-4881-414f-bd24-48d4d4bcce74"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"153b108e-4a31-4e90-b222-87c6cdaf35d7"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
   <si>
     <t>Unit</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>demand</t>
   </si>
 </sst>
 </file>
@@ -360,20 +363,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -394,15 +408,10 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -417,10 +426,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AL7" totalsRowShown="0">
-  <autoFilter ref="A1:AL7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AM7" totalsRowShown="0">
+  <autoFilter ref="A1:AM7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="39">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
@@ -457,8 +470,9 @@
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
     <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point"/>
     <tableColumn id="36" xr3:uid="{E8FC87F8-AAF9-461B-B88C-F56651B25838}" name="unit_idle_heat_rate"/>
-    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="0"/>
-    <tableColumn id="37" xr3:uid="{EE9BC032-0112-449B-9748-951DE19178CE}" name="Error messages:" dataDxfId="1">
+    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="4"/>
+    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="3"/>
+    <tableColumn id="37" xr3:uid="{EE9BC032-0112-449B-9748-951DE19178CE}" name="Error messages:" dataDxfId="2">
       <calculatedColumnFormula>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -475,7 +489,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -504,7 +518,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:J5" totalsRowShown="0">
   <autoFilter ref="A1:J5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="value_before"/>
@@ -818,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AL9"/>
+  <dimension ref="A1:AM9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AJ11" sqref="AJ11"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -848,10 +862,11 @@
     <col min="33" max="33" width="8.7265625" customWidth="1"/>
     <col min="36" max="36" width="19" customWidth="1"/>
     <col min="37" max="37" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.453125" customWidth="1"/>
+    <col min="38" max="38" width="10" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -963,11 +978,14 @@
       <c r="AK1" t="s">
         <v>76</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -988,12 +1006,13 @@
         <v>1.29</v>
       </c>
       <c r="AK2" s="3"/>
-      <c r="AL2" s="2" t="str">
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1034,12 +1053,13 @@
         <v>0.19</v>
       </c>
       <c r="AK3" s="3"/>
-      <c r="AL3" s="2" t="str">
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1071,12 +1091,13 @@
         <v>0.1</v>
       </c>
       <c r="AK4" s="3"/>
-      <c r="AL4" s="2" t="str">
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1108,12 +1129,15 @@
       <c r="AK5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AL5" s="2" t="str">
+      <c r="AL5" s="4">
+        <v>20.192799999999998</v>
+      </c>
+      <c r="AM5" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1173,12 +1197,13 @@
         <v>0.1</v>
       </c>
       <c r="AK6" s="3"/>
-      <c r="AL6" s="2" t="str">
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1210,12 +1235,13 @@
         <v>0.1</v>
       </c>
       <c r="AK7" s="3"/>
-      <c r="AL7" s="1" t="str">
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="1" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final inputs and new mapping order
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{40B4E73A-EA77-4643-B0C9-9E0954A17787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67852A7B-B52C-4561-B976-F047CB6EA960}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21882EED-8A47-4F9E-9E68-5EE208408FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -308,7 +308,7 @@
     <t>demand</t>
   </si>
   <si>
-    <t>W</t>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -424,10 +424,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -834,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AM9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AK6" sqref="AK6"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AL17" sqref="AL17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1263,7 +1259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add demand sensitivity runs
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21882EED-8A47-4F9E-9E68-5EE208408FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626D2A87-272E-4E4B-9BD0-C7BAEA0888FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AM9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AL17" sqref="AL17"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AL12" sqref="AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
add object type information into data base
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626D2A87-272E-4E4B-9BD0-C7BAEA0888FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988CC970-3AAB-42C5-B15C-77DB9C0427D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="2910" yWindow="-19350" windowWidth="28800" windowHeight="15225" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="89">
   <si>
     <t>Unit</t>
   </si>
@@ -309,6 +309,36 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Object_type</t>
+  </si>
+  <si>
+    <t>PV_plant</t>
+  </si>
+  <si>
+    <t>Electrolyzer_PEM</t>
+  </si>
+  <si>
+    <t>Methanol_plant</t>
+  </si>
+  <si>
+    <t>Electric_Steam_Boiler</t>
+  </si>
+  <si>
+    <t>hydrogen_storage</t>
+  </si>
+  <si>
+    <t>methanol_storage</t>
+  </si>
+  <si>
+    <t>power_line</t>
+  </si>
+  <si>
+    <t>hydrogen_pipeline</t>
+  </si>
+  <si>
+    <t>pipeline</t>
   </si>
 </sst>
 </file>
@@ -427,10 +457,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AM7" totalsRowShown="0">
-  <autoFilter ref="A1:AM7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AN7" totalsRowShown="0">
+  <autoFilter ref="A1:AN7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="40">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
+    <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{C03E717E-B39B-450F-A07B-8C087AA65297}" name="Output1"/>
@@ -477,10 +508,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:Y5" totalsRowShown="0">
-  <autoFilter ref="A1:Y5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:Z5" totalsRowShown="0">
+  <autoFilter ref="A1:Z5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{26B0CA71-1EA9-44CF-8E6D-31054ECA99A6}" name="Connection"/>
+    <tableColumn id="26" xr3:uid="{E67F4435-EF76-417C-B715-53719E5FB41F}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{587ADBB8-7B68-42BE-A14F-535C6116E5EA}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
@@ -511,12 +543,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:J5" totalsRowShown="0">
-  <autoFilter ref="A1:J5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:K5" totalsRowShown="0">
+  <autoFilter ref="A1:K5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="8" xr3:uid="{8C29206C-8DC6-44DB-A8D1-3D5625C277AD}" name="Object_type"/>
     <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="value_before"/>
     <tableColumn id="6" xr3:uid="{FA5F8582-61FC-4A96-9E8D-E08E92F1962D}" name="value_start"/>
     <tableColumn id="5" xr3:uid="{58DBFD58-A0D2-4B31-B639-19B1628ABAC8}" name="has_state"/>
@@ -828,422 +861,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AM9"/>
+  <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AL12" sqref="AL12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="4" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.1796875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" customWidth="1"/>
-    <col min="14" max="14" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="23" width="10.54296875" customWidth="1"/>
-    <col min="24" max="24" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="12.7265625" customWidth="1"/>
-    <col min="29" max="29" width="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11" customWidth="1"/>
-    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.7265625" customWidth="1"/>
-    <col min="36" max="36" width="19" customWidth="1"/>
-    <col min="37" max="37" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.453125" customWidth="1"/>
+    <col min="1" max="2" width="13.81640625" customWidth="1"/>
+    <col min="5" max="6" width="9.81640625" customWidth="1"/>
+    <col min="7" max="7" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1796875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" customWidth="1"/>
+    <col min="15" max="15" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="24" width="10.54296875" customWidth="1"/>
+    <col min="25" max="25" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.7265625" customWidth="1"/>
+    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11" customWidth="1"/>
+    <col min="32" max="32" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.7265625" customWidth="1"/>
+    <col min="37" max="37" width="19" customWidth="1"/>
+    <col min="38" max="38" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>76</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>77</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
         <v>38</v>
-      </c>
-      <c r="J2">
-        <v>304</v>
       </c>
       <c r="K2">
         <v>304</v>
       </c>
-      <c r="AA2">
+      <c r="L2">
+        <v>304</v>
+      </c>
+      <c r="AB2">
         <f>Table1[[#This Row],[Cap_Output1_existing]]*0.56</f>
         <v>170.24</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>1.29</v>
       </c>
-      <c r="AK2" s="3"/>
       <c r="AL2" s="3"/>
-      <c r="AM2" s="2" t="str">
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
       <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>41</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>42</v>
-      </c>
-      <c r="F3">
-        <v>52</v>
       </c>
       <c r="G3">
         <v>52</v>
       </c>
-      <c r="N3">
+      <c r="H3">
+        <v>52</v>
+      </c>
+      <c r="O3">
         <v>0.75</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>5.8500000000000002E-3</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>1.76</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>4.34</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>1.4865951742627345E-3</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>0.19</v>
       </c>
-      <c r="AK3" s="3"/>
       <c r="AL3" s="3"/>
-      <c r="AM3" s="2" t="str">
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
       <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>45</v>
-      </c>
-      <c r="J4">
-        <v>100</v>
       </c>
       <c r="K4">
         <v>100</v>
       </c>
-      <c r="X4">
+      <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="Y4">
         <v>3.6010731197896975E-3</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>3.601073119789697E-3</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>26.81</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>0.1</v>
       </c>
-      <c r="AK4" s="3"/>
       <c r="AL4" s="3"/>
-      <c r="AM4" s="2" t="str">
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
       <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>48</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>49</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>52</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>52</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>17.277901743828668</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <f>1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>0.1</v>
       </c>
-      <c r="AK5" s="3" t="s">
+      <c r="AL5" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AL5" s="4">
+      <c r="AM5" s="4">
         <v>20.192799999999998</v>
       </c>
-      <c r="AM5" s="2" t="str">
+      <c r="AN5" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
       <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>45</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>47</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>52</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>100</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>10</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0.7</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>51</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>0.5</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>0.5</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>0.5</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>0.5</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>5.1734967222388608</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <f>1/0.96</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>4.32</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>4.45</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>0.1</v>
       </c>
-      <c r="AK6" s="3"/>
       <c r="AL6" s="3"/>
-      <c r="AM6" s="2" t="str">
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="2" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
       <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>48</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>100</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>7.2437800000000002E-4</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>0.99</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>0.11929223744292237</v>
       </c>
-      <c r="AF7">
+      <c r="AG7">
         <v>1.4865951742627345E-3</v>
       </c>
-      <c r="AJ7">
+      <c r="AK7">
         <v>0.1</v>
       </c>
-      <c r="AK7" s="3"/>
       <c r="AL7" s="3"/>
-      <c r="AM7" s="1" t="str">
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="1" t="str">
         <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="C9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK2:AK7" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL7" xr:uid="{D92CB468-B7A9-4082-9B81-D3B4634F286E}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1257,134 +1311,137 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="4" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
-    <col min="10" max="10" width="1.7265625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" customWidth="1"/>
-    <col min="12" max="12" width="19" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="15.453125" customWidth="1"/>
-    <col min="14" max="14" width="19" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="10.54296875" customWidth="1"/>
-    <col min="16" max="16" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.81640625" customWidth="1"/>
-    <col min="20" max="20" width="12.7265625" customWidth="1"/>
-    <col min="21" max="21" width="12.81640625" customWidth="1"/>
-    <col min="22" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.81640625" customWidth="1"/>
+    <col min="5" max="6" width="9.81640625" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" customWidth="1"/>
+    <col min="11" max="11" width="1.7265625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" customWidth="1"/>
+    <col min="13" max="13" width="19" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" customWidth="1"/>
+    <col min="15" max="15" width="19" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="10.54296875" customWidth="1"/>
+    <col min="17" max="17" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.81640625" customWidth="1"/>
+    <col min="21" max="21" width="12.7265625" customWidth="1"/>
+    <col min="22" max="22" width="12.81640625" customWidth="1"/>
+    <col min="23" max="23" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
       <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>55</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>56</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>24</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>25</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>57</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>26</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>28</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>30</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>31</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>58</v>
       </c>
       <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
         <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
       </c>
       <c r="D2" t="s">
         <v>38</v>
       </c>
       <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>60</v>
       </c>
-      <c r="G2">
-        <v>1000</v>
-      </c>
       <c r="H2">
         <v>1000</v>
       </c>
@@ -1406,36 +1463,39 @@
       <c r="N2">
         <v>1000</v>
       </c>
-      <c r="Q2">
+      <c r="O2">
+        <v>1000</v>
+      </c>
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
       </c>
       <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
         <v>41</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>60</v>
       </c>
-      <c r="G3">
-        <v>1000</v>
-      </c>
-      <c r="I3">
+      <c r="H3">
         <v>1000</v>
       </c>
       <c r="J3">
@@ -1450,36 +1510,39 @@
       <c r="M3">
         <v>1000</v>
       </c>
-      <c r="S3">
+      <c r="N3">
+        <v>1000</v>
+      </c>
+      <c r="T3">
         <v>0.88</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>7.2835616438356163E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>63</v>
       </c>
       <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
         <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>64</v>
       </c>
       <c r="D4" t="s">
         <v>64</v>
       </c>
       <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
         <v>49</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>60</v>
       </c>
-      <c r="G4">
-        <v>1000</v>
-      </c>
-      <c r="I4">
+      <c r="H4">
         <v>1000</v>
       </c>
       <c r="J4">
@@ -1494,42 +1557,48 @@
       <c r="M4">
         <v>1000</v>
       </c>
-      <c r="Q4">
+      <c r="N4">
+        <v>1000</v>
+      </c>
+      <c r="R4">
         <v>0.99983999999999995</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>0.99983999999999995</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>1.0958904109589041E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>65</v>
       </c>
       <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
         <v>42</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>66</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>67</v>
       </c>
-      <c r="G5">
-        <v>1000</v>
-      </c>
       <c r="H5">
         <v>1000</v>
       </c>
-      <c r="K5">
+      <c r="I5">
         <v>1000</v>
       </c>
       <c r="L5">
         <v>1000</v>
       </c>
-      <c r="S5">
+      <c r="M5">
+        <v>1000</v>
+      </c>
+      <c r="T5">
         <v>1</v>
       </c>
     </row>
@@ -1545,102 +1614,112 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.81640625" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>62</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="b">
+      <c r="E2" t="b">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>5478.6764505058327</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>4.147E-2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>64</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" t="b">
+      <c r="E3" t="b">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2640</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{5D5BF415-E056-4F96-A602-1B73CD7FB1B5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{5D5BF415-E056-4F96-A602-1B73CD7FB1B5}">
       <formula1>"true, false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
align names of object types
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988CC970-3AAB-42C5-B15C-77DB9C0427D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43062FCA-C654-45A7-B219-90C9965826BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2910" yWindow="-19350" windowWidth="28800" windowHeight="15225" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
     <sheet name="Connections" sheetId="2" r:id="rId2"/>
     <sheet name="Storages" sheetId="3" r:id="rId3"/>
+    <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="CIQWBGuid" hidden="1">"56d80003-ecbe-478c-8e43-1a0c1458bc41"</definedName>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="92">
   <si>
     <t>Unit</t>
   </si>
@@ -320,18 +321,9 @@
     <t>Electrolyzer_PEM</t>
   </si>
   <si>
-    <t>Methanol_plant</t>
-  </si>
-  <si>
     <t>Electric_Steam_Boiler</t>
   </si>
   <si>
-    <t>hydrogen_storage</t>
-  </si>
-  <si>
-    <t>methanol_storage</t>
-  </si>
-  <si>
     <t>power_line</t>
   </si>
   <si>
@@ -339,6 +331,24 @@
   </si>
   <si>
     <t>pipeline</t>
+  </si>
+  <si>
+    <t>object_type</t>
+  </si>
+  <si>
+    <t>Electrolyzer_AEC</t>
+  </si>
+  <si>
+    <t>Electrolyzer_SOEC</t>
+  </si>
+  <si>
+    <t>Methanol_Plant</t>
+  </si>
+  <si>
+    <t>Methanol_storage</t>
+  </si>
+  <si>
+    <t>Hydrogen_storage</t>
   </si>
 </sst>
 </file>
@@ -559,6 +569,16 @@
     <tableColumn id="11" xr3:uid="{3C880482-B284-4120-859D-C69724716B06}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{DC155748-1945-4E24-B8A1-527B52E12445}" name="fom_cost"/>
     <tableColumn id="13" xr3:uid="{620A5657-4B04-4066-87F7-215E607C4C88}" name="vom_cost"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5F8A7EB-52A6-4AC4-94D0-FF5952E382A3}" name="Table4" displayName="Table4" ref="A1:A13" totalsRowShown="0">
+  <autoFilter ref="A1:A13" xr:uid="{E5F8A7EB-52A6-4AC4-94D0-FF5952E382A3}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{99EC3AFF-E76A-4BF2-94D0-13EEEC46286A}" name="object_type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -863,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1143,7 +1163,7 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
@@ -1186,7 +1206,7 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
@@ -1255,7 +1275,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -1306,6 +1326,18 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B6165F12-61B4-4BB9-9C06-E04D7CAF2ECE}">
+          <x14:formula1>
+            <xm:f>Drop_Down!$A$2:$A$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1314,7 +1346,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1425,7 +1457,7 @@
         <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>
@@ -1478,7 +1510,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -1525,7 +1557,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
         <v>49</v>
@@ -1575,7 +1607,7 @@
         <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>42</v>
@@ -1609,6 +1641,18 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A0E20513-1104-4B15-91FE-F5533BE8DD9A}">
+          <x14:formula1>
+            <xm:f>Drop_Down!$A$2:$A$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1616,8 +1660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1675,7 +1719,7 @@
         <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1698,7 +1742,7 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1727,5 +1771,103 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2BC2844F-319A-44D1-B1DA-7F8A5F123464}">
+          <x14:formula1>
+            <xm:f>Drop_Down!$A$2:$A$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DC79B9-9C58-497E-9FD8-D3F2239E9BDC}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A1:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix mapping bug in input data
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{43062FCA-C654-45A7-B219-90C9965826BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE4FC374-A0E5-400A-9182-C2036740AE6E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9820DBE0-1FF8-4E59-A6CC-FF3E820A7132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -464,10 +464,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -887,39 +883,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.85546875" customWidth="1"/>
-    <col min="5" max="6" width="9.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.81640625" customWidth="1"/>
+    <col min="5" max="6" width="9.81640625" customWidth="1"/>
+    <col min="7" max="7" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1796875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="21.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="24" width="10.5703125" customWidth="1"/>
-    <col min="25" max="25" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="24" width="10.54296875" customWidth="1"/>
+    <col min="25" max="25" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.7265625" customWidth="1"/>
     <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="11" customWidth="1"/>
-    <col min="32" max="32" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.7109375" customWidth="1"/>
+    <col min="32" max="32" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.7265625" customWidth="1"/>
     <col min="37" max="37" width="19" customWidth="1"/>
-    <col min="38" max="38" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.42578125" customWidth="1"/>
+    <col min="40" max="40" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1041,7 +1037,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1071,7 +1067,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1121,7 +1117,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1162,7 +1158,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1202,7 +1198,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1268,7 +1264,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1309,7 +1305,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="C9" s="1"/>
     </row>
   </sheetData>
@@ -1347,30 +1343,30 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.85546875" customWidth="1"/>
-    <col min="5" max="6" width="9.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="1" max="2" width="13.81640625" customWidth="1"/>
+    <col min="5" max="6" width="9.81640625" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" customWidth="1"/>
+    <col min="11" max="11" width="1.7265625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" customWidth="1"/>
     <col min="13" max="13" width="19" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" customWidth="1"/>
     <col min="15" max="15" width="19" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.85546875" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.54296875" customWidth="1"/>
+    <col min="17" max="17" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.81640625" customWidth="1"/>
+    <col min="21" max="21" width="12.7265625" customWidth="1"/>
+    <col min="22" max="22" width="12.81640625" customWidth="1"/>
+    <col min="23" max="23" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1450,7 +1446,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1503,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1550,7 +1546,7 @@
         <v>7.2835616438356163E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1600,7 +1596,7 @@
         <v>1.0958904109589041E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1658,26 +1654,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -1712,7 +1708,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1735,12 +1731,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1792,72 +1788,72 @@
       <selection activeCell="A13" sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Inserted Mathanol storage capcity in model data base sheet
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9820DBE0-1FF8-4E59-A6CC-FF3E820A7132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9820DBE0-1FF8-4E59-A6CC-FF3E820A7132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5842884-B168-40A4-99A7-21D5CC6D3F3E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="8540" yWindow="90" windowWidth="8250" windowHeight="9650" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -883,7 +883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -1177,6 +1177,9 @@
       <c r="H5">
         <v>52</v>
       </c>
+      <c r="K5">
+        <v>52</v>
+      </c>
       <c r="Y5">
         <v>17.277901743828668</v>
       </c>
@@ -1216,6 +1219,9 @@
       </c>
       <c r="F6" t="s">
         <v>42</v>
+      </c>
+      <c r="K6">
+        <v>52</v>
       </c>
       <c r="L6">
         <v>100</v>
@@ -1654,7 +1660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Old Version Data Base
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9820DBE0-1FF8-4E59-A6CC-FF3E820A7132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{9820DBE0-1FF8-4E59-A6CC-FF3E820A7132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C50E7B7F-27DF-41FD-9032-32F9E70F219A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"56d80003-ecbe-478c-8e43-1a0c1458bc41"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"786ba0cd-a80d-497b-9bfa-249ee8a2fc8d"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>

</xml_diff>

<commit_message>
adjust connection type in data base
change connection type for storage connections
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0965FF4-9CF7-4532-82A5-7344253B3B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912A1A6D-E052-46CD-8617-C5F8AEF52E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -883,7 +883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1525,7 +1525,7 @@
         <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -1572,7 +1572,7 @@
         <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="H4">
         <v>1000</v>

</xml_diff>

<commit_message>
working on the storage connection efficiencies
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912A1A6D-E052-46CD-8617-C5F8AEF52E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B03A51B-8A11-416C-9459-C1828BB51A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1544,6 +1544,9 @@
       </c>
       <c r="N3">
         <v>1000</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
       </c>
       <c r="T3">
         <v>0.88</v>

</xml_diff>

<commit_message>
Adjusted minimum operating point for electrolyzer
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\OneDrive - CBS - Copenhagen Business School\Documents\GitHub\Nord_H2ub\Spine_Projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B03A51B-8A11-416C-9459-C1828BB51A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"786ba0cd-a80d-497b-9bfa-249ee8a2fc8d"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"8308cfa2-248d-4de4-98dd-369dea72481e"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -883,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1108,7 +1108,7 @@
         <v>1.4865951742627345E-3</v>
       </c>
       <c r="AJ3">
-        <v>0.19</v>
+        <v>0.02</v>
       </c>
       <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
@@ -1345,13 +1345,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
     <col min="5" max="6" width="9.81640625" customWidth="1"/>
     <col min="7" max="7" width="17.1796875" customWidth="1"/>
     <col min="8" max="8" width="15.26953125" customWidth="1"/>
@@ -1793,9 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DC79B9-9C58-497E-9FD8-D3F2239E9BDC}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Prepared input for Spine
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\OneDrive - CBS - Copenhagen Business School\Documents\GitHub\Nord_H2ub\Spine_Projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD53B4C2-3F9A-4212-A4AA-3B27F8EFC481}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"8308cfa2-248d-4de4-98dd-369dea72481e"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"f4626026-1bdc-4a7b-a8fd-933727cea1bf"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>

</xml_diff>

<commit_message>
Added files from investment branch
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD53B4C2-3F9A-4212-A4AA-3B27F8EFC481}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7896CAD2-A274-4FD6-A634-6443E68047A2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="14010" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="111">
   <si>
     <t>Unit</t>
   </si>
@@ -349,13 +349,70 @@
   </si>
   <si>
     <t>Hydrogen_storage</t>
+  </si>
+  <si>
+    <t>storage_investment_variable_type</t>
+  </si>
+  <si>
+    <t>candidate_storages</t>
+  </si>
+  <si>
+    <t>storage_investment_tech_lifetime</t>
+  </si>
+  <si>
+    <t>number_of_storages</t>
+  </si>
+  <si>
+    <t>storage_investment_cost</t>
+  </si>
+  <si>
+    <t>storage_investment_variable_type_continuous</t>
+  </si>
+  <si>
+    <t>10Y</t>
+  </si>
+  <si>
+    <t>connection_investment_variable_type</t>
+  </si>
+  <si>
+    <t>candidate_connections</t>
+  </si>
+  <si>
+    <t>connection_investment_tech_lifetime</t>
+  </si>
+  <si>
+    <t>number_of_connections</t>
+  </si>
+  <si>
+    <t>connection_investment_cost</t>
+  </si>
+  <si>
+    <t>connection_investment_variable_type_continuous</t>
+  </si>
+  <si>
+    <t>unit_investment_variable_type</t>
+  </si>
+  <si>
+    <t>candidate_units</t>
+  </si>
+  <si>
+    <t>unit_investment_tech_lifetime</t>
+  </si>
+  <si>
+    <t>number_of_units</t>
+  </si>
+  <si>
+    <t>unit_investment_cost</t>
+  </si>
+  <si>
+    <t>unit_investment_variable_type_continuous</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +439,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -391,10 +460,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -403,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -413,22 +493,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <b val="0"/>
@@ -444,8 +517,37 @@
         <color rgb="FFFF0000"/>
         <name val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -467,9 +569,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AN7" totalsRowShown="0">
-  <autoFilter ref="A1:AN7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AS7" totalsRowShown="0">
+  <autoFilter ref="A1:AS7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="45">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="40" xr3:uid="{C2CFC5A4-5329-4F74-926A-18CEB18C062C}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
@@ -507,27 +609,30 @@
     <tableColumn id="23" xr3:uid="{1F97C2CD-E522-4842-8E10-F9B9566A6723}" name="vom_cost_Output2"/>
     <tableColumn id="34" xr3:uid="{7D7F0E89-0553-40E4-9D5A-219BF1741787}" name="minimum_op_point"/>
     <tableColumn id="36" xr3:uid="{E8FC87F8-AAF9-461B-B88C-F56651B25838}" name="unit_idle_heat_rate"/>
-    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="4"/>
-    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="3"/>
-    <tableColumn id="37" xr3:uid="{EE9BC032-0112-449B-9748-951DE19178CE}" name="Error messages:" dataDxfId="2">
-      <calculatedColumnFormula>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="38" xr3:uid="{957AF85B-8792-4643-A381-29FACAA69887}" name="resolution_output" dataDxfId="5"/>
+    <tableColumn id="39" xr3:uid="{BCE2350E-150B-4A7E-94BF-BB3BC7E31016}" name="demand" dataDxfId="4"/>
+    <tableColumn id="37" xr3:uid="{346F31E8-88ED-465C-B79B-8EF5B5998228}" name="unit_investment_variable_type"/>
+    <tableColumn id="41" xr3:uid="{6C055132-1EAE-464B-9586-C1CBFB93DE46}" name="candidate_units"/>
+    <tableColumn id="42" xr3:uid="{196BB49D-6206-466A-86DE-0BAB17646DAF}" name="unit_investment_tech_lifetime"/>
+    <tableColumn id="43" xr3:uid="{4079FBE2-CFC5-4BCF-9353-8F6771C73DD2}" name="number_of_units" dataDxfId="1"/>
+    <tableColumn id="44" xr3:uid="{5ABB776F-3BC0-406E-907C-4E35D2CBDA27}" name="unit_investment_cost"/>
+    <tableColumn id="45" xr3:uid="{4B3B8871-E458-49D5-BFE4-E2DD849EE6AD}" name="Error messages:" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:Z5" totalsRowShown="0">
-  <autoFilter ref="A1:Z5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:AE5" totalsRowShown="0">
+  <autoFilter ref="A1:AE5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="31">
     <tableColumn id="1" xr3:uid="{26B0CA71-1EA9-44CF-8E6D-31054ECA99A6}" name="Connection"/>
     <tableColumn id="26" xr3:uid="{E67F4435-EF76-417C-B715-53719E5FB41F}" name="Object_type"/>
     <tableColumn id="2" xr3:uid="{587ADBB8-7B68-42BE-A14F-535C6116E5EA}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -547,16 +652,21 @@
     <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_Input2"/>
     <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Output1"/>
     <tableColumn id="25" xr3:uid="{DDAFCF0A-1EF1-4B7B-9742-01F9FA7A22E5}" name="vom_cost_Output2"/>
+    <tableColumn id="27" xr3:uid="{97497B42-7369-4435-A0F6-3083BDCE5709}" name="connection_investment_variable_type"/>
+    <tableColumn id="28" xr3:uid="{477D63E9-4696-4858-8BA3-AC12DF5EA9AA}" name="candidate_connections"/>
+    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime"/>
+    <tableColumn id="30" xr3:uid="{09434E4A-7BF5-4547-9708-EA3F0F7ADC8E}" name="number_of_connections"/>
+    <tableColumn id="31" xr3:uid="{FD5F1FDC-A519-47B1-8C2A-A84CD36A8B25}" name="connection_investment_cost"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:K5" totalsRowShown="0">
-  <autoFilter ref="A1:K5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:P5" totalsRowShown="0">
+  <autoFilter ref="A1:P5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="2">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{8C29206C-8DC6-44DB-A8D1-3D5625C277AD}" name="Object_type"/>
@@ -569,6 +679,11 @@
     <tableColumn id="11" xr3:uid="{3C880482-B284-4120-859D-C69724716B06}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{DC155748-1945-4E24-B8A1-527B52E12445}" name="fom_cost"/>
     <tableColumn id="13" xr3:uid="{620A5657-4B04-4066-87F7-215E607C4C88}" name="vom_cost"/>
+    <tableColumn id="9" xr3:uid="{A8A11461-F396-4D3E-B9FC-F4D1EE9D9AA5}" name="storage_investment_variable_type"/>
+    <tableColumn id="10" xr3:uid="{CE81AD39-C6F6-4493-9451-68A39075BF6E}" name="candidate_storages"/>
+    <tableColumn id="14" xr3:uid="{58E34C8A-1B4C-437B-981D-CD4CFED1B3A8}" name="storage_investment_tech_lifetime"/>
+    <tableColumn id="15" xr3:uid="{5FF71707-8528-4768-8697-8818F4BC14D6}" name="number_of_storages"/>
+    <tableColumn id="16" xr3:uid="{8C607D2E-BC5C-4E67-8BF2-33EAD803CDBB}" name="storage_investment_cost"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -881,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AN9"/>
+  <dimension ref="A1:AS9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -912,10 +1027,10 @@
     <col min="37" max="37" width="19" customWidth="1"/>
     <col min="38" max="38" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.453125" customWidth="1"/>
+    <col min="45" max="45" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1033,11 +1148,26 @@
       <c r="AM1" t="s">
         <v>77</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1062,12 +1192,24 @@
       </c>
       <c r="AL2" s="3"/>
       <c r="AM2" s="3"/>
-      <c r="AN2" s="2" t="str">
-        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AN2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ2" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="AR2">
+        <v>560000</v>
+      </c>
+      <c r="AS2" s="2"/>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1112,12 +1254,24 @@
       </c>
       <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
-      <c r="AN3" s="2" t="str">
-        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AN3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ3" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="AR3">
+        <v>1900000</v>
+      </c>
+      <c r="AS3" s="2"/>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1153,12 +1307,24 @@
       </c>
       <c r="AL4" s="3"/>
       <c r="AM4" s="3"/>
-      <c r="AN4" s="2" t="str">
-        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AN4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO4">
+        <v>1</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ4" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="AR4">
+        <v>500000</v>
+      </c>
+      <c r="AS4" s="2"/>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1196,12 +1362,24 @@
       <c r="AM5" s="4">
         <v>20.192799999999998</v>
       </c>
-      <c r="AN5" s="2" t="str">
-        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AN5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ5" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="AR5">
+        <v>1350000</v>
+      </c>
+      <c r="AS5" s="2"/>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1265,12 +1443,24 @@
       </c>
       <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
-      <c r="AN6" s="2" t="str">
-        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AN6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO6">
+        <v>1</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ6" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="AR6">
+        <v>1350000</v>
+      </c>
+      <c r="AS6" s="2"/>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1306,12 +1496,24 @@
       </c>
       <c r="AL7" s="3"/>
       <c r="AM7" s="3"/>
-      <c r="AN7" s="1" t="str">
-        <f>IF( Table1[[#This Row],[minimum_op_point]]="", "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 1, "", IF( COUNTA(Table1[[#This Row],[Cap_Input1_existing]], Table1[[#This Row],[Cap_Input2_existing]], Table1[[#This Row],[Cap_Output1_existing]], Table1[[#This Row],[Cap_Output2_existing]]) = 0, "Capacity missing", "Too many capacities" ) ) )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AN7" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO7">
+        <v>1</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ7" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="AR7">
+        <v>150000</v>
+      </c>
+      <c r="AS7" s="2"/>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
       <c r="C9" s="1"/>
     </row>
   </sheetData>
@@ -1343,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1373,7 +1575,7 @@
     <col min="23" max="23" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1452,8 +1654,23 @@
       <c r="Z1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1505,8 +1722,23 @@
       <c r="T2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD2">
+        <v>0.1</v>
+      </c>
+      <c r="AE2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1555,8 +1787,23 @@
       <c r="V3">
         <v>7.2835616438356163E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD3">
+        <v>0.1</v>
+      </c>
+      <c r="AE3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1605,8 +1852,23 @@
       <c r="V4">
         <v>1.0958904109589041E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB4">
+        <v>1</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD4">
+        <v>0.1</v>
+      </c>
+      <c r="AE4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1636,6 +1898,21 @@
       </c>
       <c r="T5">
         <v>1</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD5">
+        <v>0.1</v>
+      </c>
+      <c r="AE5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1662,10 +1939,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L1" sqref="L1:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1683,7 +1960,7 @@
     <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -1717,8 +1994,23 @@
       <c r="K1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1740,8 +2032,23 @@
       <c r="H2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2">
+        <v>0.1</v>
+      </c>
+      <c r="P2">
+        <v>0.121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1762,6 +2069,21 @@
       </c>
       <c r="H3" t="s">
         <v>75</v>
+      </c>
+      <c r="L3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>98</v>
+      </c>
+      <c r="O3">
+        <v>0.1</v>
+      </c>
+      <c r="P3">
+        <v>1.3958682300390841E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected candidate units solar plants to 1
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7896CAD2-A274-4FD6-A634-6443E68047A2}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA7F5DCA-56B4-4639-8E42-183E1DE32637}"/>
   <bookViews>
-    <workbookView xWindow="14010" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-22815" yWindow="-21720" windowWidth="51840" windowHeight="21240" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"f4626026-1bdc-4a7b-a8fd-933727cea1bf"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"9bc45d17-43fd-4650-ba88-b8af6f587998"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -503,6 +503,17 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -537,17 +548,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -614,9 +614,9 @@
     <tableColumn id="37" xr3:uid="{346F31E8-88ED-465C-B79B-8EF5B5998228}" name="unit_investment_variable_type"/>
     <tableColumn id="41" xr3:uid="{6C055132-1EAE-464B-9586-C1CBFB93DE46}" name="candidate_units"/>
     <tableColumn id="42" xr3:uid="{196BB49D-6206-466A-86DE-0BAB17646DAF}" name="unit_investment_tech_lifetime"/>
-    <tableColumn id="43" xr3:uid="{4079FBE2-CFC5-4BCF-9353-8F6771C73DD2}" name="number_of_units" dataDxfId="1"/>
+    <tableColumn id="43" xr3:uid="{4079FBE2-CFC5-4BCF-9353-8F6771C73DD2}" name="number_of_units" dataDxfId="3"/>
     <tableColumn id="44" xr3:uid="{5ABB776F-3BC0-406E-907C-4E35D2CBDA27}" name="unit_investment_cost"/>
-    <tableColumn id="45" xr3:uid="{4B3B8871-E458-49D5-BFE4-E2DD849EE6AD}" name="Error messages:" dataDxfId="0"/>
+    <tableColumn id="45" xr3:uid="{4B3B8871-E458-49D5-BFE4-E2DD849EE6AD}" name="Error messages:" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -632,7 +632,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -666,7 +666,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:P5" totalsRowShown="0">
   <autoFilter ref="A1:P5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{8C29206C-8DC6-44DB-A8D1-3D5625C277AD}" name="Object_type"/>
@@ -998,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AS9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AQ1" sqref="AQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1196,13 +1196,13 @@
         <v>110</v>
       </c>
       <c r="AO2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP2" t="s">
         <v>98</v>
       </c>
       <c r="AQ2" s="6">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="AR2">
         <v>560000</v>
@@ -1547,8 +1547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AE5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1942,7 +1942,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:P5"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2116,7 +2116,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DC79B9-9C58-497E-9FD8-D3F2239E9BDC}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
changes in start of jupyter notebook and added outputs manually to model
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="282" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3543DFBB-342C-4D4C-AA20-3E427DB4F389}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2089195-73D9-4E30-8D90-6A7A836DD69A}"/>
   <bookViews>
-    <workbookView xWindow="28785" yWindow="-16440" windowWidth="16440" windowHeight="28440" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="104">
   <si>
     <t>Unit</t>
   </si>
@@ -351,9 +351,6 @@
     <t>storage_investment_cost</t>
   </si>
   <si>
-    <t>10Y</t>
-  </si>
-  <si>
     <t>connection_investment_tech_lifetime</t>
   </si>
   <si>
@@ -387,13 +384,7 @@
     <t>Methanol_pipeline</t>
   </si>
   <si>
-    <t>25Y</t>
-  </si>
-  <si>
-    <t>40Y</t>
-  </si>
-  <si>
-    <t>50Y</t>
+    <t>365D</t>
   </si>
 </sst>
 </file>
@@ -453,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -464,7 +455,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +614,7 @@
     <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_Input2"/>
     <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Output1"/>
     <tableColumn id="25" xr3:uid="{DDAFCF0A-1EF1-4B7B-9742-01F9FA7A22E5}" name="vom_cost_Output2"/>
-    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="0"/>
+    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="2"/>
     <tableColumn id="30" xr3:uid="{09434E4A-7BF5-4547-9708-EA3F0F7ADC8E}" name="number_of_connections"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -635,7 +625,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:N5" totalsRowShown="0">
   <autoFilter ref="A1:N5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="1">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{8C29206C-8DC6-44DB-A8D1-3D5625C277AD}" name="Object_type"/>
@@ -648,7 +638,7 @@
     <tableColumn id="11" xr3:uid="{3C880482-B284-4120-859D-C69724716B06}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{DC155748-1945-4E24-B8A1-527B52E12445}" name="fom_cost"/>
     <tableColumn id="13" xr3:uid="{620A5657-4B04-4066-87F7-215E607C4C88}" name="vom_cost"/>
-    <tableColumn id="14" xr3:uid="{58E34C8A-1B4C-437B-981D-CD4CFED1B3A8}" name="storage_investment_tech_lifetime" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{58E34C8A-1B4C-437B-981D-CD4CFED1B3A8}" name="storage_investment_tech_lifetime" dataDxfId="0"/>
     <tableColumn id="15" xr3:uid="{5FF71707-8528-4768-8697-8818F4BC14D6}" name="number_of_storages"/>
     <tableColumn id="16" xr3:uid="{8C607D2E-BC5C-4E67-8BF2-33EAD803CDBB}" name="storage_investment_cost"/>
   </tableColumns>
@@ -965,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AQ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AN25" sqref="AN25"/>
+    <sheetView topLeftCell="AJ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AP11" sqref="AP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1117,13 +1107,13 @@
         <v>77</v>
       </c>
       <c r="AN1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AO1" t="s">
         <v>95</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>96</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>97</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>36</v>
@@ -1155,10 +1145,10 @@
       <c r="AL2" s="3"/>
       <c r="AM2" s="3"/>
       <c r="AN2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AO2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="AP2" s="5">
         <v>1</v>
@@ -1211,10 +1201,10 @@
       <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
       <c r="AN3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AO3" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="AP3" s="5">
         <v>0.2</v>
@@ -1258,10 +1248,10 @@
       <c r="AL4" s="3"/>
       <c r="AM4" s="3"/>
       <c r="AN4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AO4" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="AP4" s="5">
         <v>0.2</v>
@@ -1307,10 +1297,10 @@
         <v>20.192799999999998</v>
       </c>
       <c r="AN5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AO5" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="AP5" s="5">
         <v>0.2</v>
@@ -1382,10 +1372,10 @@
       <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
       <c r="AN6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AO6" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="AP6" s="5">
         <v>0.2</v>
@@ -1429,10 +1419,10 @@
       <c r="AL7" s="3"/>
       <c r="AM7" s="3"/>
       <c r="AN7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AO7" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="AP7" s="5">
         <v>0.2</v>
@@ -1474,7 +1464,7 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+      <selection activeCell="AA2" sqref="AA2:AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1500,7 +1490,7 @@
     <col min="22" max="22" width="12.81640625" customWidth="1"/>
     <col min="23" max="24" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="35.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="35.26953125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="24.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1583,11 +1573,11 @@
       <c r="Z1" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB1" t="s">
         <v>93</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.35">
@@ -1595,7 +1585,7 @@
         <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>
@@ -1642,8 +1632,8 @@
       <c r="T2">
         <v>1</v>
       </c>
-      <c r="AA2" s="6" t="s">
-        <v>105</v>
+      <c r="AA2" t="s">
+        <v>103</v>
       </c>
       <c r="AB2">
         <v>0.1</v>
@@ -1654,7 +1644,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -1698,8 +1688,8 @@
       <c r="V3">
         <v>7.2835616438356163E-2</v>
       </c>
-      <c r="AA3" s="6" t="s">
-        <v>106</v>
+      <c r="AA3" t="s">
+        <v>103</v>
       </c>
       <c r="AB3">
         <v>0.1</v>
@@ -1710,7 +1700,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
         <v>49</v>
@@ -1754,8 +1744,8 @@
       <c r="V4">
         <v>1.0958904109589041E-2</v>
       </c>
-      <c r="AA4" s="6" t="s">
-        <v>105</v>
+      <c r="AA4" t="s">
+        <v>103</v>
       </c>
       <c r="AB4">
         <v>0.1</v>
@@ -1766,7 +1756,7 @@
         <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
         <v>42</v>
@@ -1792,8 +1782,8 @@
       <c r="T5">
         <v>1</v>
       </c>
-      <c r="AA5" s="6" t="s">
-        <v>105</v>
+      <c r="AA5" t="s">
+        <v>103</v>
       </c>
       <c r="AB5">
         <v>0.1</v>
@@ -1825,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1842,7 +1832,7 @@
     <col min="9" max="9" width="9" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -1879,7 +1869,7 @@
       <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" t="s">
         <v>89</v>
       </c>
       <c r="M1" t="s">
@@ -1911,8 +1901,8 @@
       <c r="H2" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>104</v>
+      <c r="L2" t="s">
+        <v>103</v>
       </c>
       <c r="M2">
         <v>0.1</v>
@@ -1943,8 +1933,8 @@
       <c r="H3" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>104</v>
+      <c r="L3" t="s">
+        <v>103</v>
       </c>
       <c r="M3">
         <v>0.1</v>
@@ -2044,27 +2034,27 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added units_on_cost to model
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2089195-73D9-4E30-8D90-6A7A836DD69A}"/>
+  <xr:revisionPtr revIDLastSave="312" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B5174C4-14DE-4334-B161-57A1B1895330}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -156,9 +156,6 @@
     <t>Cost_invest</t>
   </si>
   <si>
-    <t>unit_on_cost</t>
-  </si>
-  <si>
     <t>fom_cost</t>
   </si>
   <si>
@@ -385,6 +382,9 @@
   </si>
   <si>
     <t>365D</t>
+  </si>
+  <si>
+    <t>units_on_cost</t>
   </si>
 </sst>
 </file>
@@ -532,6 +532,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AQ7" totalsRowShown="0">
   <autoFilter ref="A1:AQ7" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
@@ -564,7 +568,7 @@
     <tableColumn id="20" xr3:uid="{84C680FD-12EA-4AE2-A238-57453A3D8C12}" name="Relation_In_Out"/>
     <tableColumn id="10" xr3:uid="{ACDE4024-BCA2-4145-B3BC-1A5A08F3EA7D}" name="Relation_Out_Out"/>
     <tableColumn id="11" xr3:uid="{8AEC88A1-B64A-43A2-AC89-3B27AB4ACAD7}" name="Cost_invest"/>
-    <tableColumn id="25" xr3:uid="{95F69D80-80E7-42BD-B42F-59F3C3DC485B}" name="unit_on_cost"/>
+    <tableColumn id="25" xr3:uid="{95F69D80-80E7-42BD-B42F-59F3C3DC485B}" name="units_on_cost"/>
     <tableColumn id="12" xr3:uid="{F1A83AF0-CF23-4B00-9076-4E28DF8DAFD3}" name="fom_cost"/>
     <tableColumn id="24" xr3:uid="{4D171E04-3F62-4131-BD43-B8A8D03B8530}" name="vom_cost"/>
     <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="vom_cost_Input1"/>
@@ -955,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AQ9"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AP11" sqref="AP11"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -993,7 +997,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1074,60 +1078,60 @@
         <v>26</v>
       </c>
       <c r="AC1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
         <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
       </c>
       <c r="K2">
         <v>304</v>
@@ -1145,10 +1149,10 @@
       <c r="AL2" s="3"/>
       <c r="AM2" s="3"/>
       <c r="AN2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AP2" s="5">
         <v>1</v>
@@ -1157,22 +1161,22 @@
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>41</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
       </c>
       <c r="G3">
         <v>52</v>
@@ -1201,10 +1205,10 @@
       <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
       <c r="AN3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AP3" s="5">
         <v>0.2</v>
@@ -1213,19 +1217,19 @@
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>44</v>
-      </c>
-      <c r="E4" t="s">
-        <v>45</v>
       </c>
       <c r="K4">
         <v>100</v>
@@ -1248,10 +1252,10 @@
       <c r="AL4" s="3"/>
       <c r="AM4" s="3"/>
       <c r="AN4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AP4" s="5">
         <v>0.2</v>
@@ -1260,19 +1264,19 @@
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="B5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>49</v>
       </c>
       <c r="H5">
         <v>52</v>
@@ -1291,16 +1295,16 @@
         <v>0.1</v>
       </c>
       <c r="AL5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AM5" s="4">
         <v>20.192799999999998</v>
       </c>
       <c r="AN5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AP5" s="5">
         <v>0.2</v>
@@ -1309,22 +1313,22 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
         <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>42</v>
       </c>
       <c r="K6">
         <v>52</v>
@@ -1339,7 +1343,7 @@
         <v>0.7</v>
       </c>
       <c r="P6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q6">
         <v>0.5</v>
@@ -1372,10 +1376,10 @@
       <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
       <c r="AN6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AP6" s="5">
         <v>0.2</v>
@@ -1384,19 +1388,19 @@
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7">
         <v>100</v>
@@ -1419,10 +1423,10 @@
       <c r="AL7" s="3"/>
       <c r="AM7" s="3"/>
       <c r="AN7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AO7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AP7" s="5">
         <v>0.2</v>
@@ -1496,10 +1500,10 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1514,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1532,7 +1536,7 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N1" t="s">
         <v>11</v>
@@ -1541,7 +1545,7 @@
         <v>12</v>
       </c>
       <c r="P1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q1" t="s">
         <v>23</v>
@@ -1553,54 +1557,54 @@
         <v>25</v>
       </c>
       <c r="T1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="U1" t="s">
         <v>26</v>
       </c>
       <c r="V1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" t="s">
-        <v>33</v>
-      </c>
       <c r="AA1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB1" t="s">
         <v>92</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
         <v>59</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" t="s">
-        <v>60</v>
       </c>
       <c r="H2">
         <v>1000</v>
@@ -1633,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="AA2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB2">
         <v>0.1</v>
@@ -1641,25 +1645,25 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>62</v>
-      </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H3">
         <v>1000</v>
@@ -1689,7 +1693,7 @@
         <v>7.2835616438356163E-2</v>
       </c>
       <c r="AA3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB3">
         <v>0.1</v>
@@ -1697,25 +1701,25 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H4">
         <v>1000</v>
@@ -1745,7 +1749,7 @@
         <v>1.0958904109589041E-2</v>
       </c>
       <c r="AA4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB4">
         <v>0.1</v>
@@ -1753,19 +1757,19 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
         <v>65</v>
       </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>66</v>
-      </c>
-      <c r="G5" t="s">
-        <v>67</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -1783,7 +1787,7 @@
         <v>1</v>
       </c>
       <c r="AA5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB5">
         <v>0.1</v>
@@ -1815,7 +1819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -1837,54 +1841,54 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>70</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>72</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>73</v>
-      </c>
-      <c r="H1" t="s">
-        <v>74</v>
       </c>
       <c r="I1" t="s">
         <v>26</v>
       </c>
       <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" t="s">
-        <v>29</v>
-      </c>
       <c r="L1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" t="s">
         <v>89</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>90</v>
-      </c>
-      <c r="N1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1899,10 +1903,10 @@
         <v>4.147E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M2">
         <v>0.1</v>
@@ -1913,10 +1917,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1931,10 +1935,10 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M3">
         <v>0.1</v>
@@ -1984,77 +1988,77 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted investment periods to days and removed error messages in data_prep notebook
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="312" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B5174C4-14DE-4334-B161-57A1B1895330}"/>
+  <xr:revisionPtr revIDLastSave="373" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEAA3A66-29A5-468E-9497-9C7649FC20A9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-22815" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"a941d177-e092-4f1a-a5e6-19844c7b685c"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"8c3e62b9-2db8-4eff-bc49-a7b631e6a873"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -381,10 +381,10 @@
     <t>Methanol_pipeline</t>
   </si>
   <si>
-    <t>365D</t>
-  </si>
-  <si>
     <t>units_on_cost</t>
+  </si>
+  <si>
+    <t>1Y</t>
   </si>
 </sst>
 </file>
@@ -530,10 +530,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -959,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AQ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AC7" sqref="AC7"/>
+    <sheetView topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AP25" sqref="AP25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -989,6 +985,7 @@
     <col min="38" max="38" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="30" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1078,7 +1075,7 @@
         <v>26</v>
       </c>
       <c r="AC1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AD1" t="s">
         <v>27</v>
@@ -1152,7 +1149,7 @@
         <v>96</v>
       </c>
       <c r="AO2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AP2" s="5">
         <v>1</v>
@@ -1208,7 +1205,7 @@
         <v>96</v>
       </c>
       <c r="AO3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AP3" s="5">
         <v>0.2</v>
@@ -1255,7 +1252,7 @@
         <v>96</v>
       </c>
       <c r="AO4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AP4" s="5">
         <v>0.2</v>
@@ -1304,7 +1301,7 @@
         <v>96</v>
       </c>
       <c r="AO5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AP5" s="5">
         <v>0.2</v>
@@ -1379,7 +1376,7 @@
         <v>96</v>
       </c>
       <c r="AO6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AP6" s="5">
         <v>0.2</v>
@@ -1426,7 +1423,7 @@
         <v>96</v>
       </c>
       <c r="AO7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AP7" s="5">
         <v>0.2</v>
@@ -1467,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2:AA5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1637,7 +1634,7 @@
         <v>1</v>
       </c>
       <c r="AA2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB2">
         <v>0.1</v>
@@ -1693,7 +1690,7 @@
         <v>7.2835616438356163E-2</v>
       </c>
       <c r="AA3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB3">
         <v>0.1</v>
@@ -1749,7 +1746,7 @@
         <v>1.0958904109589041E-2</v>
       </c>
       <c r="AA4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB4">
         <v>0.1</v>
@@ -1787,7 +1784,7 @@
         <v>1</v>
       </c>
       <c r="AA5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB5">
         <v>0.1</v>
@@ -1819,8 +1816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1906,7 +1903,7 @@
         <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M2">
         <v>0.1</v>
@@ -1938,7 +1935,7 @@
         <v>74</v>
       </c>
       <c r="L3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M3">
         <v>0.1</v>

</xml_diff>

<commit_message>
Updated investment lifetimes to true values
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="373" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEAA3A66-29A5-468E-9497-9C7649FC20A9}"/>
+  <xr:revisionPtr revIDLastSave="389" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E827B7E0-5DDD-4E81-B7CF-6976C000577D}"/>
   <bookViews>
-    <workbookView xWindow="-22815" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-22695" yWindow="-21600" windowWidth="25800" windowHeight="21000" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Drop_Down" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"8c3e62b9-2db8-4eff-bc49-a7b631e6a873"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"c22a6a05-0005-488b-bfe2-cbbbe086fca2"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.51.3510.3078"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="109">
   <si>
     <t>Unit</t>
   </si>
@@ -384,7 +384,22 @@
     <t>units_on_cost</t>
   </si>
   <si>
-    <t>1Y</t>
+    <t>50Y</t>
+  </si>
+  <si>
+    <t>40Y</t>
+  </si>
+  <si>
+    <t>35Y</t>
+  </si>
+  <si>
+    <t>25Y</t>
+  </si>
+  <si>
+    <t>30Y</t>
+  </si>
+  <si>
+    <t>20Y</t>
   </si>
 </sst>
 </file>
@@ -955,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AQ9"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AP25" sqref="AP25"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1149,7 +1164,7 @@
         <v>96</v>
       </c>
       <c r="AO2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AP2" s="5">
         <v>1</v>
@@ -1205,7 +1220,7 @@
         <v>96</v>
       </c>
       <c r="AO3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AP3" s="5">
         <v>0.2</v>
@@ -1252,7 +1267,7 @@
         <v>96</v>
       </c>
       <c r="AO4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="AP4" s="5">
         <v>0.2</v>
@@ -1301,7 +1316,7 @@
         <v>96</v>
       </c>
       <c r="AO5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="AP5" s="5">
         <v>0.2</v>
@@ -1376,7 +1391,7 @@
         <v>96</v>
       </c>
       <c r="AO6" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="AP6" s="5">
         <v>0.2</v>
@@ -1423,7 +1438,7 @@
         <v>96</v>
       </c>
       <c r="AO7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="AP7" s="5">
         <v>0.2</v>
@@ -1464,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z33" sqref="Z33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1634,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="AA2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AB2">
         <v>0.1</v>
@@ -1784,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="AA5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AB5">
         <v>0.1</v>
@@ -1816,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1903,7 +1918,7 @@
         <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="M2">
         <v>0.1</v>
@@ -1935,7 +1950,7 @@
         <v>74</v>
       </c>
       <c r="L3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="M3">
         <v>0.1</v>

</xml_diff>

<commit_message>
adjust initial units in input data
for the investment the initial capacity should be 0 (if not otherwise specified).
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/methanol/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/methanol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="389" documentId="13_ncr:1_{96B3803C-A484-4494-82AB-C52E20681BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E827B7E0-5DDD-4E81-B7CF-6976C000577D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D954787A-120F-4E9B-9D31-96F6A5AD2E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22695" yWindow="-21600" windowWidth="25800" windowHeight="21000" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -970,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AQ9"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AN12" sqref="AN12"/>
+    <sheetView topLeftCell="AG1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AP11" sqref="AP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1167,7 +1167,7 @@
         <v>105</v>
       </c>
       <c r="AP2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ2" s="2"/>
     </row>
@@ -1223,7 +1223,7 @@
         <v>106</v>
       </c>
       <c r="AP3" s="5">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AQ3" s="2"/>
     </row>
@@ -1270,7 +1270,7 @@
         <v>108</v>
       </c>
       <c r="AP4" s="5">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AQ4" s="2"/>
     </row>
@@ -1319,7 +1319,7 @@
         <v>107</v>
       </c>
       <c r="AP5" s="5">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AQ5" s="2"/>
     </row>
@@ -1394,7 +1394,7 @@
         <v>107</v>
       </c>
       <c r="AP6" s="5">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AQ6" s="2"/>
     </row>
@@ -1441,7 +1441,7 @@
         <v>108</v>
       </c>
       <c r="AP7" s="5">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AQ7" s="2"/>
     </row>
@@ -1480,7 +1480,7 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1652,7 +1652,7 @@
         <v>104</v>
       </c>
       <c r="AB2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.35">
@@ -1708,7 +1708,7 @@
         <v>103</v>
       </c>
       <c r="AB3">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.35">
@@ -1764,7 +1764,7 @@
         <v>103</v>
       </c>
       <c r="AB4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
@@ -1802,7 +1802,7 @@
         <v>104</v>
       </c>
       <c r="AB5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1831,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1921,7 +1921,7 @@
         <v>106</v>
       </c>
       <c r="M2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>0.121</v>
@@ -1953,7 +1953,7 @@
         <v>106</v>
       </c>
       <c r="M3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>1.3958682300390841E-4</v>

</xml_diff>